<commit_message>
Nueva version, rodadas las imágenes, y eliminado errores
</commit_message>
<xml_diff>
--- a/results_cec2015.pdf.xlsx
+++ b/results_cec2015.pdf.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="DECC-G" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,14 +18,13 @@
     <sheet name="IHDELS_orig" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="CC-CMA-ES" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="CC-CMA-ES_orig" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="IHDELS_restart_t01" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="646">
   <si>
     <t>1.2e5</t>
   </si>
@@ -2359,7 +2358,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -3309,254 +3308,6 @@
         <v>645</v>
       </c>
       <c r="J32" s="5"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D16"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="n">
-        <v>72400</v>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>0.327</v>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>9.1E-025</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="n">
-        <v>1810</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>1720</v>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>1640</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="n">
-        <v>20.2</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>20.2</v>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>20.2</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="n">
-        <v>46300000000</v>
-      </c>
-      <c r="C5" s="4" t="n">
-        <v>4130000000</v>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>309000000</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4" t="n">
-        <v>73600000</v>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>24500000</v>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>13400000</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="4" t="n">
-        <v>1050000</v>
-      </c>
-      <c r="C7" s="4" t="n">
-        <v>1040000</v>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>1040000</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4" t="n">
-        <v>913000000</v>
-      </c>
-      <c r="C8" s="4" t="n">
-        <v>25400000</v>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>17400</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="4" t="n">
-        <v>543000000000000</v>
-      </c>
-      <c r="C9" s="4" t="n">
-        <v>46700000000000</v>
-      </c>
-      <c r="D9" s="4" t="n">
-        <v>2570000000000</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4" t="n">
-        <v>755000000</v>
-      </c>
-      <c r="C10" s="4" t="n">
-        <v>646000000</v>
-      </c>
-      <c r="D10" s="4" t="n">
-        <v>479000000</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="4" t="n">
-        <v>93700000</v>
-      </c>
-      <c r="C11" s="4" t="n">
-        <v>93000000</v>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>92000000</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="4" t="n">
-        <v>34500000000</v>
-      </c>
-      <c r="C12" s="4" t="n">
-        <v>800000000</v>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>17600000</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="4" t="n">
-        <v>2510</v>
-      </c>
-      <c r="C13" s="4" t="n">
-        <v>1170</v>
-      </c>
-      <c r="D13" s="4" t="n">
-        <v>72.6</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4" t="n">
-        <v>12400000000</v>
-      </c>
-      <c r="C14" s="4" t="n">
-        <v>719000000</v>
-      </c>
-      <c r="D14" s="4" t="n">
-        <v>2150000</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="4" t="n">
-        <v>139000000000</v>
-      </c>
-      <c r="C15" s="4" t="n">
-        <v>564000000</v>
-      </c>
-      <c r="D15" s="4" t="n">
-        <v>12500000</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="4" t="n">
-        <v>80200000</v>
-      </c>
-      <c r="C16" s="4" t="n">
-        <v>13900000</v>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>1690000</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>